<commit_message>
Added the data for B=0.05
</commit_message>
<xml_diff>
--- a/LeakageModel/Data/Dickson_N=3.xlsx
+++ b/LeakageModel/Data/Dickson_N=3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\Working-Projects\LeakageModel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DD61DB7-3A34-4DD8-AEC4-78408B7AEDA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38606E11-7398-4E8E-BAFA-BC641C0908D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{76FF834E-ACC5-487B-A317-ACFF6B2A0525}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{76FF834E-ACC5-487B-A317-ACFF6B2A0525}"/>
   </bookViews>
   <sheets>
     <sheet name="Dickson_Real_N=3" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="16">
   <si>
     <t>f (MHz)</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>eta</t>
+  </si>
+  <si>
+    <t>T = 0.05</t>
+  </si>
+  <si>
+    <t>B = 0.05</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -421,20 +433,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E2E590-B460-48F4-A335-17410187DBEC}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -445,7 +457,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -465,7 +477,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>50</v>
       </c>
@@ -486,7 +498,7 @@
         <v>0.87484034788955123</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100</v>
       </c>
@@ -507,7 +519,7 @@
         <v>0.87489167919356259</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>200</v>
       </c>
@@ -528,7 +540,7 @@
         <v>0.87490531583930731</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>300</v>
       </c>
@@ -549,7 +561,7 @@
         <v>0.87491115623810112</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>400</v>
       </c>
@@ -570,12 +582,12 @@
         <v>0.87493492811105611</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -586,7 +598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -603,18 +615,24 @@
         <v>4</v>
       </c>
       <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>50</v>
       </c>
       <c r="B14">
-        <v>15.547000000000001</v>
+        <v>15.625</v>
       </c>
       <c r="C14">
-        <v>68.114000000000004</v>
+        <v>67.95</v>
       </c>
       <c r="D14">
         <v>3.5</v>
@@ -623,19 +641,25 @@
         <v>1</v>
       </c>
       <c r="F14">
+        <v>0.01</v>
+      </c>
+      <c r="G14">
+        <v>0.01</v>
+      </c>
+      <c r="H14">
         <f>B14*D14/(C14*E14)</f>
-        <v>0.79887394661890365</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.80481972038263427</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>100</v>
       </c>
       <c r="B15">
-        <v>26.427</v>
+        <v>26.571000000000002</v>
       </c>
       <c r="C15">
-        <v>117.46</v>
+        <v>117.17</v>
       </c>
       <c r="D15">
         <v>3.5</v>
@@ -644,19 +668,25 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <f t="shared" ref="F15:F18" si="1">B15*D15/(C15*E15)</f>
-        <v>0.78745530393325391</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.01</v>
+      </c>
+      <c r="G15">
+        <v>0.01</v>
+      </c>
+      <c r="H15">
+        <f>B15*D15/(C15*E15)</f>
+        <v>0.79370572672185713</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>200</v>
       </c>
       <c r="B16">
-        <v>33.164999999999999</v>
+        <v>33.438000000000002</v>
       </c>
       <c r="C16">
-        <v>156.09</v>
+        <v>155.5</v>
       </c>
       <c r="D16">
         <v>3.5</v>
@@ -665,19 +695,25 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
-        <v>0.7436575052854123</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.01</v>
+      </c>
+      <c r="G16">
+        <v>0.01</v>
+      </c>
+      <c r="H16">
+        <f>B16*D16/(C16*E16)</f>
+        <v>0.7526237942122187</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>300</v>
       </c>
       <c r="B17">
-        <v>33.634</v>
+        <v>34.078000000000003</v>
       </c>
       <c r="C17">
-        <v>169.85</v>
+        <v>168.89</v>
       </c>
       <c r="D17">
         <v>3.5</v>
@@ -686,19 +722,25 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <f t="shared" si="1"/>
-        <v>0.6930762437444804</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.01</v>
+      </c>
+      <c r="G17">
+        <v>0.01</v>
+      </c>
+      <c r="H17">
+        <f>B17*D17/(C17*E17)</f>
+        <v>0.70621706436141884</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>400</v>
       </c>
       <c r="B18">
-        <v>32.670999999999999</v>
+        <v>33.235999999999997</v>
       </c>
       <c r="C18">
-        <v>177.56</v>
+        <v>176.37</v>
       </c>
       <c r="D18">
         <v>3.5</v>
@@ -707,8 +749,155 @@
         <v>1</v>
       </c>
       <c r="F18">
+        <v>0.01</v>
+      </c>
+      <c r="G18">
+        <v>0.01</v>
+      </c>
+      <c r="H18">
+        <f>B18*D18/(C18*E18)</f>
+        <v>0.65955661393661047</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>50</v>
+      </c>
+      <c r="B24">
+        <v>12.265000000000001</v>
+      </c>
+      <c r="C24">
+        <v>76.5</v>
+      </c>
+      <c r="D24">
+        <v>3.5</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f>B24*D24/(C24*E24)</f>
+        <v>0.56114379084967325</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>100</v>
+      </c>
+      <c r="B25">
+        <v>19.567</v>
+      </c>
+      <c r="C25">
+        <v>133.11000000000001</v>
+      </c>
+      <c r="D25">
+        <v>3.5</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ref="F25:F28" si="1">B25*D25/(C25*E25)</f>
+        <v>0.51449553001277126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>200</v>
+      </c>
+      <c r="B26">
+        <v>18.942</v>
+      </c>
+      <c r="C26">
+        <v>185.43</v>
+      </c>
+      <c r="D26">
+        <v>3.5</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
         <f t="shared" si="1"/>
-        <v>0.64399921153412931</v>
+        <v>0.35753114382785955</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>300</v>
+      </c>
+      <c r="B27">
+        <v>12.17</v>
+      </c>
+      <c r="C27">
+        <v>213.21</v>
+      </c>
+      <c r="D27">
+        <v>3.5</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>0.19977956005815861</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>400</v>
+      </c>
+      <c r="B28">
+        <v>3.976</v>
+      </c>
+      <c r="C28">
+        <v>235.2</v>
+      </c>
+      <c r="D28">
+        <v>3.5</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>5.9166666666666673E-2</v>
       </c>
     </row>
   </sheetData>
@@ -718,10 +907,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DE6631-70A1-49EE-9A42-D4EA1B5334C5}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,145 +1017,286 @@
         <v>1</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>15.598000000000001</v>
+      </c>
+      <c r="C12">
+        <v>67.91</v>
+      </c>
+      <c r="D12">
+        <v>3.5</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f>B12*D12/(C12*E12)</f>
+        <v>0.80390222353114427</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>100</v>
+      </c>
+      <c r="B13">
+        <v>26.56</v>
+      </c>
+      <c r="C13">
+        <v>117.035</v>
+      </c>
+      <c r="D13">
+        <v>3.5</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13:F16" si="0">B13*D13/(C13*E13)</f>
+        <v>0.7942923057205109</v>
+      </c>
+    </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14">
+        <v>200</v>
+      </c>
+      <c r="B14">
+        <v>33.340000000000003</v>
+      </c>
+      <c r="C14">
+        <v>155.34</v>
+      </c>
+      <c r="D14">
+        <v>3.5</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.75119093601133002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>300</v>
+      </c>
+      <c r="B15">
+        <v>33.93</v>
+      </c>
+      <c r="C15">
+        <v>168.77</v>
+      </c>
+      <c r="D15">
+        <v>3.5</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.70364993778515128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>400</v>
+      </c>
+      <c r="B16">
+        <v>33.04</v>
+      </c>
+      <c r="C16">
+        <v>176.16</v>
+      </c>
+      <c r="D16">
+        <v>3.5</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.65644868301544057</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
         <v>2</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D20" t="s">
         <v>3</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E20" t="s">
         <v>4</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F20" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>50</v>
-      </c>
-      <c r="B17">
-        <v>15.598000000000001</v>
-      </c>
-      <c r="C17">
-        <v>67.89</v>
-      </c>
-      <c r="D17">
-        <v>3.5</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <f>B17*D17/(C17*E17)</f>
-        <v>0.80413904846074535</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>100</v>
-      </c>
-      <c r="B18">
-        <v>26.5</v>
-      </c>
-      <c r="C18">
-        <v>117.035</v>
-      </c>
-      <c r="D18">
-        <v>3.5</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <f t="shared" ref="F18:F21" si="0">B18*D18/(C18*E18)</f>
-        <v>0.79249797069252792</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>200</v>
-      </c>
-      <c r="B19">
-        <v>33.197000000000003</v>
-      </c>
-      <c r="C19">
-        <v>154.77000000000001</v>
-      </c>
-      <c r="D19">
-        <v>3.5</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>0.75072365445499778</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>300</v>
-      </c>
-      <c r="B20">
-        <v>33.758000000000003</v>
-      </c>
-      <c r="C20">
-        <v>168.023</v>
-      </c>
-      <c r="D20">
-        <v>3.5</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>0.70319539586842283</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
+        <v>50</v>
+      </c>
+      <c r="B21">
+        <v>12.24</v>
+      </c>
+      <c r="C21">
+        <v>76.466999999999999</v>
+      </c>
+      <c r="D21">
+        <v>3.5</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <f>B21*D21/(C21*E21)</f>
+        <v>0.56024167287849669</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>100</v>
+      </c>
+      <c r="B22">
+        <v>19.515999999999998</v>
+      </c>
+      <c r="C22">
+        <v>133.03</v>
+      </c>
+      <c r="D22">
+        <v>3.5</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ref="F22:F25" si="1">B22*D22/(C22*E22)</f>
+        <v>0.51346312861760501</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>200</v>
+      </c>
+      <c r="B23">
+        <v>18.838999999999999</v>
+      </c>
+      <c r="C23">
+        <v>185.35</v>
+      </c>
+      <c r="D23">
+        <v>3.5</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0.35574049096304289</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>300</v>
+      </c>
+      <c r="B24">
+        <v>12.015000000000001</v>
+      </c>
+      <c r="C24">
+        <v>213.05</v>
+      </c>
+      <c r="D24">
+        <v>3.5</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>0.19738324337010091</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>400</v>
       </c>
-      <c r="B21">
-        <v>32.851999999999997</v>
-      </c>
-      <c r="C21">
-        <v>175.4</v>
-      </c>
-      <c r="D21">
-        <v>3.5</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>0.65554161915621423</v>
+      <c r="B25">
+        <v>3.7549999999999999</v>
+      </c>
+      <c r="C25">
+        <v>235.02</v>
+      </c>
+      <c r="D25">
+        <v>3.5</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>5.5920772700195728E-2</v>
       </c>
     </row>
   </sheetData>
@@ -975,6 +1305,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CE776A79FE4A6F4D843C4553C31CC3EB" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cc552f40ec9790170e21c3285891af83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="c9839d10-9e81-42c9-8514-76f9beb7498e" xmlns:ns4="83519e31-e1c4-478c-9e81-109dae184f8c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f1e554566fda3fbb5fc391cde33249cf" ns3:_="" ns4:_="">
     <xsd:import namespace="c9839d10-9e81-42c9-8514-76f9beb7498e"/>
@@ -1171,22 +1516,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA25CD61-B673-46CF-8EC5-3945D8EFCBAE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="c9839d10-9e81-42c9-8514-76f9beb7498e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="83519e31-e1c4-478c-9e81-109dae184f8c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A03C0FC-82DB-4FC0-86D4-1291DE411A73}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB3D10F7-1BFC-4348-9AE7-1CF33FE3BE63}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1203,29 +1558,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A03C0FC-82DB-4FC0-86D4-1291DE411A73}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA25CD61-B673-46CF-8EC5-3945D8EFCBAE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="c9839d10-9e81-42c9-8514-76f9beb7498e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="83519e31-e1c4-478c-9e81-109dae184f8c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>